<commit_message>
added a remove button for the food ordered
</commit_message>
<xml_diff>
--- a/backend/daily_reports_1.xlsx
+++ b/backend/daily_reports_1.xlsx
@@ -450,7 +450,7 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>428</v>
+        <v>760</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -459,7 +459,7 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>428</v>
+        <v>760</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed styling for delete buttons
</commit_message>
<xml_diff>
--- a/backend/daily_reports_1.xlsx
+++ b/backend/daily_reports_1.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -26,9 +26,6 @@
   </si>
   <si>
     <t>Net Profit</t>
-  </si>
-  <si>
-    <t>2023-08-15</t>
   </si>
   <si>
     <t>2023-08-16</t>
@@ -408,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -433,7 +430,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>620</v>
+        <v>205</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -442,24 +439,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>760</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>760</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the last 2 buttons to add employee and supply cost
</commit_message>
<xml_diff>
--- a/backend/daily_reports_1.xlsx
+++ b/backend/daily_reports_1.xlsx
@@ -430,16 +430,16 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>205</v>
+        <v>395</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E2">
-        <v>205</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>